<commit_message>
Atualização do cronograma das atividades do Bootcamp Inter
</commit_message>
<xml_diff>
--- a/Cronograma do Bootcamp/Cronograma Bootcamp Inter.xlsx
+++ b/Cronograma do Bootcamp/Cronograma Bootcamp Inter.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea2e232a8603278b/Desktop/DIO Cursos/meu-primeiro-projeto/Cronograma do Bootcamp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{6B9781A5-E1FA-4679-BFEA-C1C6B24F35B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,163 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Atividades</t>
+  </si>
+  <si>
+    <t>Boas-Vindas ao Bootcamp Inter Frontend Developer</t>
+  </si>
+  <si>
+    <t>Concluido</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Bootcamp Inter Frontend</t>
+  </si>
+  <si>
+    <t>Lógica de Programação Essencial</t>
+  </si>
+  <si>
+    <t>Básico</t>
+  </si>
+  <si>
+    <t>Aprenda o que são Estrutura de Dados e Algoritmos</t>
+  </si>
+  <si>
+    <t>Intermediário</t>
+  </si>
+  <si>
+    <t>Introdução ao Git e ao GitHub</t>
+  </si>
+  <si>
+    <t>Projetos ágeis com SCRUM</t>
+  </si>
+  <si>
+    <t>Criando seu Primeiro Repositório no GitHub para compartilhar seu progresso</t>
+  </si>
+  <si>
+    <t>Mentoria #1: Aula Inaugural - Bootcamp Inter Frontend Developer</t>
+  </si>
+  <si>
+    <t>Mentoria #2: Como Ser o próximo contratado pelo INTER</t>
+  </si>
+  <si>
+    <t>Introdução a criação de websites com HTML5 e CSS3</t>
+  </si>
+  <si>
+    <t>Contruindo páginas para internet com Bootstrap</t>
+  </si>
+  <si>
+    <t>IDE Instalação e configuração (Visual Studio Code)</t>
+  </si>
+  <si>
+    <t>Introdução ao JavaScript</t>
+  </si>
+  <si>
+    <t>Sintaxe Básica em JavaScript</t>
+  </si>
+  <si>
+    <t>Sintaxe e Operadores</t>
+  </si>
+  <si>
+    <t>Variáveis e tipos</t>
+  </si>
+  <si>
+    <t>Funções</t>
+  </si>
+  <si>
+    <t>Coleções</t>
+  </si>
+  <si>
+    <t>Debugging e Error Handling</t>
+  </si>
+  <si>
+    <t>JavaScript Assíncrono</t>
+  </si>
+  <si>
+    <t>Orientação a objetos</t>
+  </si>
+  <si>
+    <t>Map, Filter e Reduce</t>
+  </si>
+  <si>
+    <t>Manipulando a D.O.M com JavaScript</t>
+  </si>
+  <si>
+    <t>Resolvendo Desafios de código em JavaScript</t>
+  </si>
+  <si>
+    <t>Mentoria #3: Como resolver os desafios do código</t>
+  </si>
+  <si>
+    <t>Programando com JS</t>
+  </si>
+  <si>
+    <t>Recriando a Interface do Netflix</t>
+  </si>
+  <si>
+    <t>Avançado</t>
+  </si>
+  <si>
+    <t>SQL Server - Criando suas primeiras consultas</t>
+  </si>
+  <si>
+    <t>Modelando um banco de dados na prática com SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server: Boas práticas em bancos relacionais </t>
+  </si>
+  <si>
+    <t>Introdução ao ReactJS</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de aplicação para internet com ReactJS</t>
+  </si>
+  <si>
+    <t>Trabalhando com Componentes em React</t>
+  </si>
+  <si>
+    <t>Introdução aos React Hooks</t>
+  </si>
+  <si>
+    <t>trabalhandocom States &amp; Effects no ReacjtJS</t>
+  </si>
+  <si>
+    <t>Mentoria #4: desenvolvendo um frontend de uma aplicação web com experts do INTER</t>
+  </si>
+  <si>
+    <t>Introdução a APIs e métodos HTTP</t>
+  </si>
+  <si>
+    <t>Instalando e configurando seu ambiente NODE.JS</t>
+  </si>
+  <si>
+    <t>Explorando o estilo arquitetural REST com NODE.JS</t>
+  </si>
+  <si>
+    <t>NODE.JS com bancos de dados relacionais (SQL)</t>
+  </si>
+  <si>
+    <t>Microsserviços e integrações com Node.JS</t>
+  </si>
+  <si>
+    <t>Mentoria #5: Consumindo APIs feitas em NODE.JS em um Frontend com Experts do Inter</t>
+  </si>
+  <si>
+    <t>Integrando um Backend em NODE.JS com um frontend em react para um E-Commerce</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +210,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +495,378 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>